<commit_message>
push pc to laptop
</commit_message>
<xml_diff>
--- a/report/ReportLeads.xlsx
+++ b/report/ReportLeads.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0457903-9397-4622-B127-74A416865A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="CRM_Leads" sheetId="1" r:id="rId1"/>
-    <sheet name="EDM_Leads" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="CRM_Leads" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="EDM_Leads" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="95">
   <si>
     <t>FullName</t>
   </si>
@@ -49,24 +45,274 @@
   </si>
   <si>
     <t>dateStamp</t>
+  </si>
+  <si>
+    <t>test cdp 1</t>
+  </si>
+  <si>
+    <t>le@gmail.com</t>
+  </si>
+  <si>
+    <t>0905212346</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>cdp</t>
+  </si>
+  <si>
+    <t>test cpd 4</t>
+  </si>
+  <si>
+    <t>boo@gmail.com</t>
+  </si>
+  <si>
+    <t>0900900901</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>lehoangvu1209@gmail.com</t>
+  </si>
+  <si>
+    <t>0905293836</t>
+  </si>
+  <si>
+    <t>eeee</t>
+  </si>
+  <si>
+    <t>test cdp 6</t>
+  </si>
+  <si>
+    <t>bood@gmail.com</t>
+  </si>
+  <si>
+    <t>0900900902</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 9:13:52 am</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Vy</t>
+  </si>
+  <si>
+    <t>boodevil99@gmail.com</t>
+  </si>
+  <si>
+    <t>0905293830</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 9:25:06 am</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Vũ test cdp</t>
+  </si>
+  <si>
+    <t>lehoangvu2222@gmail.com</t>
+  </si>
+  <si>
+    <t>0905293222</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 11:07:05 am</t>
+  </si>
+  <si>
+    <t>test cdp 11</t>
+  </si>
+  <si>
+    <t>lehoangvy@gmail.com</t>
+  </si>
+  <si>
+    <t>0905293987</t>
+  </si>
+  <si>
+    <t>12346789</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 11:13:19 am</t>
+  </si>
+  <si>
+    <t>Hoàng Vũ test</t>
+  </si>
+  <si>
+    <t>0909090909</t>
+  </si>
+  <si>
+    <t>Tét</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 12:52:58 pm</t>
+  </si>
+  <si>
+    <t>Hoàng Vũ Lê tét</t>
+  </si>
+  <si>
+    <t>leho9@gmail.com</t>
+  </si>
+  <si>
+    <t>0908070605</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 12:55:26 pm</t>
+  </si>
+  <si>
+    <t>test cdp 17</t>
+  </si>
+  <si>
+    <t>bood9@gmail.com</t>
+  </si>
+  <si>
+    <t>0905939461</t>
+  </si>
+  <si>
+    <t>hgf</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:10:47 pm</t>
+  </si>
+  <si>
+    <t>dd dfds</t>
+  </si>
+  <si>
+    <t>fds@ttt.com</t>
+  </si>
+  <si>
+    <t>gdf</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:19:13 pm</t>
+  </si>
+  <si>
+    <t>rrrrr r e re</t>
+  </si>
+  <si>
+    <t>retwww@gmail.com</t>
+  </si>
+  <si>
+    <t>0905345345</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:23:35 pm</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Vũ test cdp 111</t>
+  </si>
+  <si>
+    <t>sdf@tr.com</t>
+  </si>
+  <si>
+    <t>0905293123</t>
+  </si>
+  <si>
+    <t>test cdp ;ần cuối</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 4:11:42 pm</t>
+  </si>
+  <si>
+    <t>test cpd demo thử</t>
+  </si>
+  <si>
+    <t>leh111@gmail.com</t>
+  </si>
+  <si>
+    <t>0905293333</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>June 3rd 2021, 2:01:14 pm</t>
+  </si>
+  <si>
+    <t>June 3rd 2021, 2:01:59 pm</t>
+  </si>
+  <si>
+    <t>1234567@gmail.com</t>
+  </si>
+  <si>
+    <t>0901111111</t>
+  </si>
+  <si>
+    <t>test cdp</t>
+  </si>
+  <si>
+    <t>June 3rd 2021, 2:06:38 pm</t>
+  </si>
+  <si>
+    <t>Ha Nam</t>
+  </si>
+  <si>
+    <t>hanangnam@yahoo.com</t>
+  </si>
+  <si>
+    <t>0903606773</t>
+  </si>
+  <si>
+    <t>Nhận mặt bằng căn hộ và báo giá</t>
+  </si>
+  <si>
+    <t>June 4th 2021, 7:02:16 am</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 9:02:27 am</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 9:03:01 am</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 11:01:23 am</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 11:05:27 am</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:08:52 pm</t>
+  </si>
+  <si>
+    <t>4r</t>
+  </si>
+  <si>
+    <t>er@c.com</t>
+  </si>
+  <si>
+    <t>0923423234</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:17:35 pm</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:18:16 pm</t>
+  </si>
+  <si>
+    <t>June 2nd 2021, 3:18:33 pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -430,14 +676,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -474,23 +715,636 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>30</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>30</v>
+      </c>
+      <c r="J18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,9 +1375,292 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2">
+        <v>-10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>-10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <v>-10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>-10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <v>-10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5">
+        <v>-10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>-10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>-10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7">
+        <v>-10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8">
+        <v>-10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>-10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9">
+        <v>-10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>-10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>